<commit_message>
working 10-q + press release
</commit_message>
<xml_diff>
--- a/kpi_vector_langchain.xlsx
+++ b/kpi_vector_langchain.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,7 +563,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0001689548-23-000044</t>
+          <t>0001689548-22-000111</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>major depressive disorder</t>
+          <t>Major Depressive Disorder</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Announced</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>The study did not achieve statistical significance on its primary or any secondary endpoints.</t>
+          <t>The study evaluating the efficacy and safety of PRAX-114 for monotherapy treatment of major depressive disorder did not achieve statistical significance on the primary endpoint or on any secondary endpoints.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -623,12 +623,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>The study did not achieve statistical significance on any secondary endpoints.</t>
+          <t>Did not achieve statistical significance on any secondary endpoints.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Monotherapy treatment</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>No clinical benefit demonstrated.</t>
+          <t>No statistical significance on efficacy endpoints.</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -685,27 +685,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0001689548-25-000040</t>
+          <t>0001689548-22-000111</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ulixacaltamide</t>
+          <t>PRAX-222</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>essential tremor</t>
+          <t>Neurological Disorders</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Phase 3</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Essential 3 clinical trials</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -715,17 +715,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Expected</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2024H2</t>
+          <t>April 2022</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Topline results are expected from the Phase 3 clinical trials.</t>
+          <t>The FDA placed a clinical hold on the Investigational New Drug (IND) application for the study of PRAX-222 in April 2022. A letter with additional information was received in May 2022. Communication with the FDA indicated that the IND could be cleared upon submission of documentation related to a completed 13-week non-human primate toxicology study. The company submitted the requested documentation.</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -740,7 +740,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Clinical Hold Placed; IND submission updated</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -765,12 +765,12 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>US</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -790,12 +790,12 @@
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>Topline</t>
+          <t>Regulatory Update</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>Ongoing</t>
+          <t>not specified</t>
         </is>
       </c>
     </row>
@@ -807,27 +807,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0001689548-24-000060</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PRAX-628</t>
+          <t>ulixacaltamide</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Photo-Paroxysmal Response</t>
+          <t>Essential Tremor</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Phase 2a</t>
+          <t>Phase 3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Photo-Paroxysmal Response study</t>
+          <t>Essential 3 (Study 1)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -837,22 +837,22 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Announced</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2024Q1</t>
+          <t>February 2025</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Positive results announced from the study.</t>
+          <t>Results of a pre-planned interim analysis of Study 1 by the Independent Data Monitoring Committee (IDMC) recommended that the study be stopped for futility, as the results were unlikely to meet the primary efficacy endpoint. The company decided to continue both Study 1 and Study 2 to completion.</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Futility</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -907,17 +907,17 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Positive results observed.</t>
+          <t>Results for Study 1 were unlikely to meet the primary efficacy endpoint.</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>Topline</t>
+          <t>Interim</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Ongoing</t>
         </is>
       </c>
     </row>
@@ -929,27 +929,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0001689548-24-000060</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>PRAX-628</t>
+          <t>ulixacaltamide</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>focal onset seizures</t>
+          <t>Essential Tremor</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Phase 3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>first of two efficacy studies</t>
+          <t>Essential 3 (Study 1 and Study 2)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -959,17 +959,17 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Expected</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2025Q3</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Plan to initiate the first of two efficacy studies in the second half of 2024, with topline results expected in 2025.</t>
+          <t>Topline results for both Study 1 and Study 2 are expected. The decision about whether the data supports the submission of an NDA will be made after analyzing the final results for both studies.</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Ongoing</t>
         </is>
       </c>
     </row>
@@ -1051,17 +1051,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0001689548-24-000060</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PRAX-628</t>
+          <t>vomatrigine</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>focal onset seizures</t>
+          <t>Epilepsy</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>second PRAX-628 efficacy study</t>
+          <t>Photo-Paroxysmal Response (PPR) study</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1081,22 +1081,22 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Expected</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2026H1</t>
+          <t>2024Q1</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Plan to initiate a second efficacy study in the first half of 2025, with topline results expected in the first half of 2026.</t>
+          <t>Positive results were announced from the Photo-Paroxysmal Response (PPR) study.</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1151,17 +1151,17 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Positive results were observed.</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Topline</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>Planned</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1173,27 +1173,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0001689548-25-000040</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PRAX-562</t>
+          <t>vomatrigine</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SCN2A-DEE and SCN8A-DEE</t>
+          <t>Epilepsy</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Phase 2</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EMBOLD study</t>
+          <t>EMPOWER study</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Expected</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Topline results expected for both cohorts.</t>
+          <t>An observational study of vomatrigine in patients with epilepsy was initiated.</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Observational</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>Topline</t>
+          <t>not specified</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
@@ -1295,17 +1295,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0001689548-24-000060</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>elsunersen</t>
+          <t>vomatrigine</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Focal Onset Seizures or Generalized Epilepsy</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>EMBRAVE study Part 1</t>
+          <t>RADIANT</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1325,17 +1325,17 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Announced</t>
+          <t>E</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2023Q4</t>
+          <t>Mid-year 2025</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Results were shared from Part 1 of the study.</t>
+          <t>The first efficacy study, an open label eight-week study in patients with focal onset seizures or generalized epilepsy, is currently enrolling with topline results expected by mid-year 2025.</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>not specified</t>
+          <t>Open label eight-week study</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1400,12 +1400,12 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>Interim</t>
+          <t>Topline</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Enrolling</t>
         </is>
       </c>
     </row>
@@ -1417,117 +1417,849 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0001689548-25-000040</t>
+          <t>0001689548-25-000058</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>vomatrigine</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Focal Onset Seizures</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>POWER1 study</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2025H2</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>A double-blind, placebo-controlled, 12-week study was initiated in focal onset seizures in the fourth quarter of 2024, with topline results expected in the second half of 2025.</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Double-blind, placebo-controlled, 12-week study</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Placebo</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Topline</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Praxis Precision Medicines Inc</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0001689548-25-000058</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>vomatrigine</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Epilepsy</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>POWER2 study</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2025H2</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Planning to begin enrollment in a third efficacy study, POWER2, in the second half of 2025.</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Praxis Precision Medicines Inc</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0001689548-25-000058</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>relutrigine</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Epilepsy</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>EMBOLD study</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2024Q3</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Positive topline results were announced from the first cohort of the EMBOLD study. Enrollment for the second cohort has been initiated.</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Positive topline results for Cohort 1.</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Topline</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Praxis Precision Medicines Inc</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0001689548-25-000058</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>relutrigine</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Epilepsy</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>EMBOLD study (second cohort)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2026H1</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Enrollment for the second cohort has been initiated, with topline results expected no later than the first half of 2026.</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>Topline</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>Enrolling</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Praxis Precision Medicines Inc</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0001689548-25-000058</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>relutrigine</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Developmental and Epileptic Encephalopathies (DEE)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>EMERALD study</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Mid-2025</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Plan to initiate the EMERALD study in a broader DEE patient population in mid-2025.</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>Planned</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Praxis Precision Medicines Inc</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0001689548-25-000058</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>elsunersen</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Pivotal</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>The company is currently completing multiple global regulatory interactions in anticipation of starting the pivotal phase of the program.</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Regulatory interactions ongoing for pivotal phase</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>global</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>not specified</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Neurological Disorders</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>EMBRAVE study Part 1</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2023Q4</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Results from Part 1 of the EMBRAVE study were shared in the fourth quarter of 2023. The company has initiated the first arm of its global confirmatory study in Brazil.</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
         <is>
           <t>Ongoing</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Praxis Precision Medicines Inc</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0001689548-25-000058</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>elsunersen</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Neurological Disorders</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Pivotal phase</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>EMBRAVE study (second cohort of global confirmatory study)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2026H1</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Currently enrolling the second cohort of the EMBRAVE study in Brazil. Multiple global regulatory interactions are being completed to further expand the pivotal phase of the program later in 2024. Topline results for the second cohort are expected in the first half of 2026.</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Global regulatory interactions (to expand pivotal phase)</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Global confirmatory study</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Brazil; Global</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>not specified</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Topline</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>Enrolling</t>
         </is>
       </c>
     </row>

</xml_diff>